<commit_message>
Fixed services (process per batch), modified dashboard
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_preparation_v3_8_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_preparation_v3_8_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4463040-ECCA-9946-893D-6B6C604FDC85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6BB98F-2104-FA4B-B80A-1CBABA999219}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38140" yWindow="2720" windowWidth="37280" windowHeight="18360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library Batch" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="1665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="1665">
   <si>
     <t>Library Preparation Template</t>
   </si>
@@ -5887,7 +5887,9 @@
       <c r="F11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="J11" s="1" t="s">
         <v>37</v>
@@ -7746,7 +7748,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F11:F19 G12:G47</xm:sqref>
+          <xm:sqref>F11:F19 G11:G47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -7800,7 +7802,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>M11 B11 G11:J11</xm:sqref>
+          <xm:sqref>M11 B11 H11:J11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7812,7 +7814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O480"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>